<commit_message>
Assignment - brands and products
</commit_message>
<xml_diff>
--- a/Excel/Project-1(Depreciation-Calculator-Excel).xlsx
+++ b/Excel/Project-1(Depreciation-Calculator-Excel).xlsx
@@ -1,27 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CoachX\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93237944-3613-4697-A178-431E7A84693B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="12420" windowHeight="4590" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="2" r:id="rId1"/>
     <sheet name="Depreciation Calculator" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Windows User</author>
     <author>MD</author>
   </authors>
   <commentList>
-    <comment ref="D9" authorId="0">
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -35,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D15" authorId="1">
+    <comment ref="D15" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
       <text>
         <r>
           <rPr>
@@ -49,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D21" authorId="0">
+    <comment ref="D21" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
       <text>
         <r>
           <rPr>
@@ -133,7 +152,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00_ ;[Red]\-[$$-409]#,##0.00\ "/>
     <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00"/>
@@ -351,34 +370,34 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="4"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -391,6 +410,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -413,7 +435,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -505,7 +533,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="TextBox 4"/>
+        <xdr:cNvPr id="5" name="TextBox 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -691,7 +725,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -750,9 +790,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -790,7 +830,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -862,7 +902,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1035,16 +1075,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="AB19" sqref="AB19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="1" max="1" width="9.109375" customWidth="1"/>
   </cols>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1053,270 +1093,276 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="79.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="3.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="1"/>
+    <col min="1" max="1" width="3.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="79.88671875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="19.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="1"/>
     <col min="7" max="7" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.7109375" style="1"/>
+    <col min="8" max="16384" width="8.6640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="9.9499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="9.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="9"/>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
       <c r="E1" s="9"/>
     </row>
-    <row r="2" spans="1:5" ht="36.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="37.799999999999997" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="9"/>
-      <c r="B2" s="17"/>
-      <c r="C2" s="15" t="s">
+      <c r="B2" s="18"/>
+      <c r="C2" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="15"/>
+      <c r="D2" s="16"/>
       <c r="E2" s="9"/>
     </row>
-    <row r="3" spans="1:5" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="25.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="16" t="s">
+      <c r="B3" s="19"/>
+      <c r="C3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="16"/>
+      <c r="D3" s="17"/>
       <c r="E3" s="9"/>
     </row>
-    <row r="4" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="9"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
       <c r="E4" s="9"/>
     </row>
-    <row r="5" spans="1:5" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="25.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="9"/>
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
       <c r="E5" s="9"/>
     </row>
-    <row r="6" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="9"/>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="20"/>
+      <c r="C6" s="13"/>
       <c r="D6" s="10">
         <v>450000</v>
       </c>
       <c r="E6" s="9"/>
     </row>
-    <row r="7" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="20"/>
+      <c r="C7" s="13"/>
       <c r="D7" s="10">
         <v>50000</v>
       </c>
       <c r="E7" s="9"/>
     </row>
-    <row r="8" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="9"/>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="13"/>
+      <c r="D8" s="4">
+        <f>D6+D7</f>
+        <v>500000</v>
+      </c>
       <c r="E8" s="9"/>
     </row>
-    <row r="9" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="9"/>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="20"/>
+      <c r="C9" s="13"/>
       <c r="D9" s="10">
         <v>50000</v>
       </c>
       <c r="E9" s="9"/>
     </row>
-    <row r="10" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="9"/>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="20"/>
+      <c r="C10" s="13"/>
       <c r="D10" s="11">
         <v>10</v>
       </c>
       <c r="E10" s="9"/>
     </row>
-    <row r="11" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="9"/>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="14"/>
-      <c r="D11" s="4" t="str">
+      <c r="C11" s="15"/>
+      <c r="D11" s="4">
         <f>IF(D8="", "", SLN($D$8,$D$9,$D$10))</f>
-        <v/>
+        <v>45000</v>
       </c>
       <c r="E11" s="9"/>
     </row>
-    <row r="12" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="9"/>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="14"/>
-      <c r="D12" s="6" t="str">
+      <c r="C12" s="15"/>
+      <c r="D12" s="6">
         <f>IFERROR(D11/D8,"")</f>
-        <v/>
+        <v>0.09</v>
       </c>
       <c r="E12" s="9"/>
     </row>
-    <row r="13" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="9"/>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="3" t="str">
+      <c r="C13" s="13"/>
+      <c r="D13" s="3">
         <f>IF(D8="", "", D11*D10)</f>
-        <v/>
+        <v>450000</v>
       </c>
       <c r="E13" s="9"/>
     </row>
-    <row r="14" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="9"/>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="3" t="str">
+      <c r="C14" s="13"/>
+      <c r="D14" s="3">
         <f>IF(D8="", "", D8-D13)</f>
-        <v/>
+        <v>50000</v>
       </c>
       <c r="E14" s="9"/>
     </row>
-    <row r="15" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="9"/>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="3" t="str">
+      <c r="C15" s="13"/>
+      <c r="D15" s="3">
         <f>IF(D8="", "", D9-D14)</f>
-        <v/>
+        <v>0</v>
       </c>
       <c r="E15" s="9"/>
     </row>
-    <row r="16" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
       <c r="B16" s="5"/>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="9"/>
     </row>
-    <row r="17" spans="1:5" ht="27" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="25.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="9"/>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
+      <c r="C17" s="14"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="9"/>
     </row>
-    <row r="18" spans="1:5" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="18.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="9"/>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="14"/>
+      <c r="C18" s="15"/>
       <c r="D18" s="10">
         <v>450000</v>
       </c>
       <c r="E18" s="9"/>
     </row>
-    <row r="19" spans="1:5" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="18.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9"/>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="14"/>
+      <c r="C19" s="15"/>
       <c r="D19" s="10">
         <v>50000</v>
       </c>
       <c r="E19" s="9"/>
     </row>
-    <row r="20" spans="1:5" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="18.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="9"/>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="14"/>
-      <c r="D20" s="4"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="4">
+        <f>D18+D19</f>
+        <v>500000</v>
+      </c>
       <c r="E20" s="9"/>
     </row>
-    <row r="21" spans="1:5" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="18.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="9"/>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="14"/>
+      <c r="C21" s="15"/>
       <c r="D21" s="10">
         <v>50000</v>
       </c>
       <c r="E21" s="9"/>
     </row>
-    <row r="22" spans="1:5" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="18.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="9"/>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="14"/>
+      <c r="C22" s="15"/>
       <c r="D22" s="11">
         <v>10</v>
       </c>
       <c r="E22" s="9"/>
     </row>
-    <row r="23" spans="1:5" ht="18.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="18.899999999999999" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A23" s="9"/>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="6" t="str">
+      <c r="C23" s="20"/>
+      <c r="D23" s="6">
         <f>IF(D20="","",1-(D21/D20)^(1/D22))</f>
-        <v/>
+        <v>0.20567176527571851</v>
       </c>
       <c r="E23" s="9"/>
     </row>
-    <row r="24" spans="1:5" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="24" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="9"/>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
       <c r="E24" s="9"/>
     </row>
-    <row r="25" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="9"/>
       <c r="B25" s="7" t="s">
         <v>7</v>
@@ -1329,153 +1375,170 @@
       </c>
       <c r="E25" s="9"/>
     </row>
-    <row r="26" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
       <c r="B26" s="2">
         <v>1</v>
       </c>
-      <c r="C26" s="8" t="str">
+      <c r="C26" s="8">
         <f>IFERROR(IF(D26&gt;$D$21, (D26*$D$23), ""),"")</f>
-        <v/>
-      </c>
-      <c r="D26" s="8"/>
+        <v>102835.88263785925</v>
+      </c>
+      <c r="D26" s="8">
+        <f>D8</f>
+        <v>500000</v>
+      </c>
       <c r="E26" s="9"/>
     </row>
-    <row r="27" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
       <c r="B27" s="2">
         <v>2</v>
       </c>
-      <c r="C27" s="8" t="str">
+      <c r="C27" s="8">
         <f t="shared" ref="C27:C45" si="0">IFERROR(IF(D27&gt;$D$21, (D27*$D$23), ""),"")</f>
-        <v/>
-      </c>
-      <c r="D27" s="8" t="str">
+        <v>81685.445122044126</v>
+      </c>
+      <c r="D27" s="8">
         <f t="shared" ref="D27:D45" si="1">IFERROR(D26-C26, "")</f>
-        <v/>
+        <v>397164.11736214074</v>
       </c>
       <c r="E27" s="9"/>
     </row>
-    <row r="28" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="9"/>
       <c r="B28" s="2">
         <v>3</v>
       </c>
-      <c r="C28" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D28" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="C28" s="8">
+        <f t="shared" si="0"/>
+        <v>64885.05542646048</v>
+      </c>
+      <c r="D28" s="8">
+        <f t="shared" si="1"/>
+        <v>315478.67224009661</v>
       </c>
       <c r="E28" s="9"/>
     </row>
-    <row r="29" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="9"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D29" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="B29" s="2">
+        <v>4</v>
+      </c>
+      <c r="C29" s="8">
+        <f t="shared" si="0"/>
+        <v>51540.031536887516</v>
+      </c>
+      <c r="D29" s="8">
+        <f t="shared" si="1"/>
+        <v>250593.61681363612</v>
       </c>
       <c r="E29" s="9"/>
     </row>
-    <row r="30" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="9"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D30" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="B30" s="2">
+        <v>5</v>
+      </c>
+      <c r="C30" s="8">
+        <f t="shared" si="0"/>
+        <v>40939.70226832966</v>
+      </c>
+      <c r="D30" s="8">
+        <f t="shared" si="1"/>
+        <v>199053.58527674861</v>
       </c>
       <c r="E30" s="9"/>
     </row>
-    <row r="31" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="9"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D31" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="B31" s="2">
+        <v>6</v>
+      </c>
+      <c r="C31" s="8">
+        <f t="shared" si="0"/>
+        <v>32519.561432939961</v>
+      </c>
+      <c r="D31" s="8">
+        <f t="shared" si="1"/>
+        <v>158113.88300841895</v>
       </c>
       <c r="E31" s="9"/>
     </row>
-    <row r="32" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="9"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D32" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="B32" s="2">
+        <v>7</v>
+      </c>
+      <c r="C32" s="8">
+        <f t="shared" si="0"/>
+        <v>25831.205827035024</v>
+      </c>
+      <c r="D32" s="8">
+        <f t="shared" si="1"/>
+        <v>125594.321575479</v>
       </c>
       <c r="E32" s="9"/>
     </row>
-    <row r="33" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A33" s="9"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D33" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="B33" s="2">
+        <v>8</v>
+      </c>
+      <c r="C33" s="8">
+        <f t="shared" si="0"/>
+        <v>20518.456125388308</v>
+      </c>
+      <c r="D33" s="8">
+        <f t="shared" si="1"/>
+        <v>99763.115748443975</v>
       </c>
       <c r="E33" s="9"/>
     </row>
-    <row r="34" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="9"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D34" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="B34" s="2">
+        <v>9</v>
+      </c>
+      <c r="C34" s="8">
+        <f t="shared" si="0"/>
+        <v>16298.389033347312</v>
+      </c>
+      <c r="D34" s="8">
+        <f t="shared" si="1"/>
+        <v>79244.659623055661</v>
       </c>
       <c r="E34" s="9"/>
     </row>
-    <row r="35" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="9"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="8" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D35" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="B35" s="2">
+        <v>10</v>
+      </c>
+      <c r="C35" s="8">
+        <f t="shared" si="0"/>
+        <v>12946.27058970836</v>
+      </c>
+      <c r="D35" s="8">
+        <f t="shared" si="1"/>
+        <v>62946.270589708351</v>
       </c>
       <c r="E35" s="9"/>
     </row>
-    <row r="36" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="9"/>
       <c r="B36" s="2"/>
       <c r="C36" s="8" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="D36" s="8" t="str">
-        <f t="shared" si="1"/>
-        <v/>
+      <c r="D36" s="8">
+        <f t="shared" si="1"/>
+        <v>49999.999999999993</v>
       </c>
       <c r="E36" s="9"/>
     </row>
-    <row r="37" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="9"/>
       <c r="B37" s="2"/>
       <c r="C37" s="8" t="str">
@@ -1488,7 +1551,7 @@
       </c>
       <c r="E37" s="9"/>
     </row>
-    <row r="38" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9"/>
       <c r="B38" s="2"/>
       <c r="C38" s="8" t="str">
@@ -1501,7 +1564,7 @@
       </c>
       <c r="E38" s="9"/>
     </row>
-    <row r="39" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9"/>
       <c r="B39" s="2"/>
       <c r="C39" s="8" t="str">
@@ -1514,7 +1577,7 @@
       </c>
       <c r="E39" s="9"/>
     </row>
-    <row r="40" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="9"/>
       <c r="B40" s="2"/>
       <c r="C40" s="8" t="str">
@@ -1527,7 +1590,7 @@
       </c>
       <c r="E40" s="9"/>
     </row>
-    <row r="41" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="9"/>
       <c r="B41" s="2"/>
       <c r="C41" s="8" t="str">
@@ -1540,7 +1603,7 @@
       </c>
       <c r="E41" s="9"/>
     </row>
-    <row r="42" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="9"/>
       <c r="B42" s="2"/>
       <c r="C42" s="8" t="str">
@@ -1553,7 +1616,7 @@
       </c>
       <c r="E42" s="9"/>
     </row>
-    <row r="43" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="9"/>
       <c r="B43" s="2"/>
       <c r="C43" s="8" t="str">
@@ -1566,7 +1629,7 @@
       </c>
       <c r="E43" s="9"/>
     </row>
-    <row r="44" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="9"/>
       <c r="B44" s="2"/>
       <c r="C44" s="8" t="str">
@@ -1579,7 +1642,7 @@
       </c>
       <c r="E44" s="9"/>
     </row>
-    <row r="45" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="19.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="9"/>
       <c r="B45" s="2"/>
       <c r="C45" s="8" t="str">
@@ -1592,7 +1655,7 @@
       </c>
       <c r="E45" s="9"/>
     </row>
-    <row r="46" spans="1:5" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="18.600000000000001" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A46" s="9"/>
       <c r="B46" s="9"/>
       <c r="C46" s="9"/>
@@ -1601,6 +1664,20 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="C3:D3"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B5:D5"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="B10:C10"/>
@@ -1609,20 +1686,6 @@
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.19685039370078741" right="0.19685039370078741" top="0.19685039370078741" bottom="0.19685039370078741" header="0.31496062992125984" footer="0.31496062992125984"/>

</xml_diff>